<commit_message>
added report write to clearCartItem()
</commit_message>
<xml_diff>
--- a/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -49,31 +49,40 @@
     <t xml:space="preserve">login</t>
   </si>
   <si>
+    <t xml:space="preserve">Multi line items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“ ”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
     <t xml:space="preserve">productCatalogPage</t>
   </si>
   <si>
     <t xml:space="preserve">productDetailPage</t>
   </si>
   <si>
+    <t xml:space="preserve">clearCartItems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“161 162 45”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Listing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“431 53 551 561 562”</t>
+  </si>
+  <si>
     <t xml:space="preserve">cartCheck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“161 162 45”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Listing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“431 53 551 561 562”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YES</t>
   </si>
   <si>
     <t xml:space="preserve">COD Order</t>
@@ -111,7 +120,7 @@
     <t xml:space="preserve">filters in test</t>
   </si>
   <si>
-    <t xml:space="preserve">“ ”</t>
+    <t xml:space="preserve">checking cartitemclear</t>
   </si>
 </sst>
 </file>
@@ -121,7 +130,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -162,6 +171,13 @@
       <color rgb="FF000000"/>
       <name val="Monospace"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -207,7 +223,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,6 +241,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -249,23 +269,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7091836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="17.6377551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.3367346938776"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.53571428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,140 +321,162 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>11</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
confirmation() added to script package
</commit_message>
<xml_diff>
--- a/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -52,10 +52,7 @@
     <t xml:space="preserve">Multi line items</t>
   </si>
   <si>
-    <t xml:space="preserve">“ ”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YES</t>
+    <t xml:space="preserve">“ 431 53”</t>
   </si>
   <si>
     <t xml:space="preserve">productCatalogPage</t>
@@ -120,7 +117,19 @@
     <t xml:space="preserve">filters in test</t>
   </si>
   <si>
-    <t xml:space="preserve">checking cartitemclear</t>
+    <t xml:space="preserve">“ ”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checking checkout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">confirmationPage</t>
   </si>
 </sst>
 </file>
@@ -272,21 +281,20 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.53571428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.39795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -328,155 +336,167 @@
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>17</v>
       </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>22</v>
-      </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="G6" s="0" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="0" t="s">
         <v>23</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>10</v>
-      </c>
       <c r="C9" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="B10" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>14</v>
+        <v>34</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new breadCrum() added to script
</commit_message>
<xml_diff>
--- a/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Action2</t>
   </si>
   <si>
-    <t xml:space="preserve">Log In</t>
+    <t xml:space="preserve">Login at Home page</t>
   </si>
   <si>
     <t xml:space="preserve">“1434”</t>
@@ -49,40 +49,52 @@
     <t xml:space="preserve">login</t>
   </si>
   <si>
-    <t xml:space="preserve">Multi line items</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“ 431 53”</t>
+    <t xml:space="preserve">logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login at product Listing page</t>
   </si>
   <si>
     <t xml:space="preserve">productCatalogPage</t>
   </si>
   <si>
+    <t xml:space="preserve">Login at Product detail Page</t>
+  </si>
+  <si>
     <t xml:space="preserve">productDetailPage</t>
   </si>
   <si>
+    <t xml:space="preserve">Login at checkout page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkoutLogin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login in search page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“161 162 45”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding multple products from listing page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“431 53 551 561 562”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cartCheck</t>
+  </si>
+  <si>
     <t xml:space="preserve">clearCartItems</t>
   </si>
   <si>
-    <t xml:space="preserve">Search Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“161 162 45”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Product Listing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“431 53 551 561 562”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cartCheck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COD Order</t>
+    <t xml:space="preserve">Adding product from search page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Placing COD order</t>
   </si>
   <si>
     <t xml:space="preserve">“1434 431 53 551 561 562 
@@ -95,6 +107,9 @@
     <t xml:space="preserve">orderCOD</t>
   </si>
   <si>
+    <t xml:space="preserve">confirmationPage</t>
+  </si>
+  <si>
     <t xml:space="preserve">Checking Filters</t>
   </si>
   <si>
@@ -105,6 +120,18 @@
     <t xml:space="preserve">applyFilters</t>
   </si>
   <si>
+    <t xml:space="preserve">checking Breadcrums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">breadCrums</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emailing Reports</t>
   </si>
   <si>
@@ -123,13 +150,13 @@
     <t xml:space="preserve">checking checkout</t>
   </si>
   <si>
-    <t xml:space="preserve">“”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">confirmationPage</t>
+    <t xml:space="preserve">checkingconfirmation page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multi line items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“ 431 53”</t>
   </si>
 </sst>
 </file>
@@ -278,23 +305,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="5.39795918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.4897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.2908163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.05102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7908163265306"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -327,176 +360,368 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="2"/>
+      <c r="P2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="3"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="2"/>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="3"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="2"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="0" t="s">
+      <c r="G5" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="3"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="2"/>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="B6" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="0" t="s">
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="0" t="s">
+      <c r="K7" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="K9" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="0" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="B10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="0" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="K14" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C15" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>35</v>
+      <c r="E15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
logout()- modified by adding'/' to HOME URL
</commit_message>
<xml_diff>
--- a/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">“1434”</t>
   </si>
   <si>
-    <t xml:space="preserve">NO</t>
+    <t xml:space="preserve">YES</t>
   </si>
   <si>
     <t xml:space="preserve">login</t>
@@ -120,22 +120,25 @@
     <t xml:space="preserve">applyFilters</t>
   </si>
   <si>
-    <t xml:space="preserve">checking Breadcrums</t>
+    <t xml:space="preserve">checking Breadcrums in listing page</t>
   </si>
   <si>
     <t xml:space="preserve">“”</t>
   </si>
   <si>
-    <t xml:space="preserve">YES</t>
-  </si>
-  <si>
     <t xml:space="preserve">breadCrums</t>
   </si>
   <si>
+    <t xml:space="preserve">checking Beadcrum in productview page</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emailing Reports</t>
   </si>
   <si>
     <t xml:space="preserve">“007”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO</t>
   </si>
   <si>
     <t xml:space="preserve">emailReport</t>
@@ -305,29 +308,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P16"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.2908163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.05102040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.61224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.2551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -565,8 +568,11 @@
       <c r="K9" s="0" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L9" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>29</v>
       </c>
@@ -591,79 +597,61 @@
         <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>38</v>
+        <v>35</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>39</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="C14" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="J14" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -674,7 +662,7 @@
         <v>33</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -685,42 +673,80 @@
       <c r="F15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="J15" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="K15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="0" t="s">
+      <c r="L15" s="0" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H16" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="B17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" s="2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added util folder with config file and all referenced jar files
</commit_message>
<xml_diff>
--- a/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="48">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -52,16 +52,19 @@
     <t xml:space="preserve">logout</t>
   </si>
   <si>
+    <t xml:space="preserve">Login at Product detail Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productCatalogPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productDetailPage</t>
+  </si>
+  <si>
     <t xml:space="preserve">Login at product Listing page</t>
   </si>
   <si>
-    <t xml:space="preserve">productCatalogPage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login at Product detail Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">productDetailPage</t>
+    <t xml:space="preserve">NO</t>
   </si>
   <si>
     <t xml:space="preserve">Login at checkout page</t>
@@ -92,6 +95,18 @@
   </si>
   <si>
     <t xml:space="preserve">Adding product from search page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checking Breadcrums in product catalog page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">breadCrums</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checking Beadcrum in productdetail page</t>
   </si>
   <si>
     <t xml:space="preserve">Placing COD order</t>
@@ -120,27 +135,12 @@
     <t xml:space="preserve">applyFilters</t>
   </si>
   <si>
-    <t xml:space="preserve">checking Breadcrums in listing page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">breadCrums</t>
-  </si>
-  <si>
-    <t xml:space="preserve">checking Beadcrum in productview page</t>
-  </si>
-  <si>
     <t xml:space="preserve">Emailing Reports</t>
   </si>
   <si>
     <t xml:space="preserve">“007”</t>
   </si>
   <si>
-    <t xml:space="preserve">NO</t>
-  </si>
-  <si>
     <t xml:space="preserve">emailReport</t>
   </si>
   <si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t xml:space="preserve">“ 431 53”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My orders</t>
+  </si>
+  <si>
+    <t xml:space="preserve">myAccounts</t>
   </si>
 </sst>
 </file>
@@ -308,29 +314,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.61224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.1377551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="22.0051020408163"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.2551020408163"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0663265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -357,7 +364,7 @@
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -381,19 +388,21 @@
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="G3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2"/>
       <c r="H3" s="5"/>
       <c r="I3" s="3"/>
       <c r="M3" s="4"/>
@@ -402,26 +411,24 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
+      <c r="C4" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>9</v>
       </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="5"/>
       <c r="I4" s="3"/>
       <c r="M4" s="4"/>
@@ -430,22 +437,22 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>9</v>
@@ -458,16 +465,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>8</v>
@@ -478,163 +485,163 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" s="0" t="s">
+      <c r="I11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="2" t="s">
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>7</v>
+      <c r="C12" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>39</v>
@@ -648,10 +655,10 @@
         <v>41</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -659,10 +666,10 @@
         <v>42</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -671,25 +678,25 @@
         <v>11</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,10 +704,10 @@
         <v>43</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -709,19 +716,19 @@
         <v>11</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,22 +739,39 @@
         <v>45</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
config file added and util package added
</commit_message>
<xml_diff>
--- a/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="49">
   <si>
     <t xml:space="preserve">Test Scenario</t>
   </si>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">“1434”</t>
   </si>
   <si>
-    <t xml:space="preserve">YES</t>
+    <t xml:space="preserve">NO</t>
   </si>
   <si>
     <t xml:space="preserve">login</t>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t xml:space="preserve">Login at product Listing page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NO</t>
   </si>
   <si>
     <t xml:space="preserve">Login at checkout page</t>
@@ -166,6 +163,12 @@
   </si>
   <si>
     <t xml:space="preserve">myAccounts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checking checkout page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
   </si>
 </sst>
 </file>
@@ -314,30 +317,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.0663265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.5459183673469"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.2244897959184"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,7 +419,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>11</v>
@@ -437,13 +439,13 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>11</v>
@@ -452,7 +454,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" s="0" t="s">
         <v>9</v>
@@ -465,16 +467,16 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>18</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>8</v>
@@ -485,57 +487,57 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="0" t="s">
+      <c r="K7" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4"/>
@@ -543,56 +545,56 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="B11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="C11" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>11</v>
@@ -601,75 +603,75 @@
         <v>12</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="J11" s="0" t="s">
+      <c r="K11" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="K11" s="0" t="s">
-        <v>33</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="C13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>41</v>
-      </c>
       <c r="C14" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -687,27 +689,27 @@
         <v>12</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J15" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="L15" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -719,27 +721,27 @@
         <v>12</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H16" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="I16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J16" s="0" t="s">
         <v>32</v>
-      </c>
-      <c r="J16" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="C17" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>11</v>
@@ -754,24 +756,41 @@
         <v>12</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>47</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
structure modified for sake of building jar file and also config file
</commit_message>
<xml_diff>
--- a/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
+++ b/java/Hybrid/bin/com/styletag/testcases/TestSuit.xlsx
@@ -43,46 +43,49 @@
     <t xml:space="preserve">“1434”</t>
   </si>
   <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login at Product detail Page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productCatalogPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">productDetailPage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login at product Listing page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login at checkout page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checkoutLogin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login in search page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“161 162 45”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding multple products from listing page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">“431 53 551 561 562”</t>
+  </si>
+  <si>
     <t xml:space="preserve">NO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login at Product detail Page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">productCatalogPage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">productDetailPage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login at product Listing page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login at checkout page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">checkoutLogin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Login in search page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“161 162 45”</t>
-  </si>
-  <si>
-    <t xml:space="preserve">search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adding multple products from listing page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">“431 53 551 561 562”</t>
   </si>
   <si>
     <t xml:space="preserve">cartCheck</t>
@@ -166,9 +169,6 @@
   </si>
   <si>
     <t xml:space="preserve">checking checkout page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YES</t>
   </si>
 </sst>
 </file>
@@ -325,21 +325,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.5255102040816"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.1224489795918"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -493,7 +494,7 @@
         <v>20</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>11</v>
@@ -514,15 +515,15 @@
         <v>12</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>17</v>
@@ -537,7 +538,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4"/>
@@ -545,10 +546,10 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>7</v>
@@ -557,73 +558,73 @@
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>21</v>
-      </c>
       <c r="I11" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="L11" s="0" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>7</v>
@@ -632,46 +633,46 @@
         <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -689,27 +690,27 @@
         <v>12</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K15" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>8</v>
@@ -721,27 +722,27 @@
         <v>12</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>11</v>
@@ -756,41 +757,41 @@
         <v>12</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>